<commit_message>
TP4 falta solo un generador, n-partito
</commit_message>
<xml_diff>
--- a/TP4/Documentacion/Planilla de Metricas.xlsx
+++ b/TP4/Documentacion/Planilla de Metricas.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmartin\Desktop\progra\pa-group\TP4\Documentacion\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Métricas" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -785,53 +780,95 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="166" fontId="2" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="6" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -841,235 +878,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="6" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color theme="0"/>
@@ -1116,7 +931,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-AR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1360,7 +1175,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1395,7 +1210,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1607,7 +1422,7 @@
   <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,29 +1440,29 @@
       <c r="B1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="57"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="63"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -1673,15 +1488,15 @@
       <c r="E3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="82"/>
       <c r="O3" s="14"/>
       <c r="P3" s="9"/>
     </row>
@@ -1700,15 +1515,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C4),ISBLANK(D4)),"Completar",IF(D4&gt;=C4,D4-C4,"Error")),"Error")</f>
         <v>2.083333333333337E-2</v>
       </c>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="66"/>
-      <c r="M4" s="66"/>
-      <c r="N4" s="66"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="64"/>
+      <c r="M4" s="64"/>
+      <c r="N4" s="64"/>
       <c r="O4" s="15"/>
       <c r="P4" s="11"/>
     </row>
@@ -1732,12 +1547,12 @@
     </row>
     <row r="6" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="57"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="63"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -1763,15 +1578,15 @@
       <c r="E7" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="65"/>
-      <c r="K7" s="65"/>
-      <c r="L7" s="65"/>
-      <c r="M7" s="65"/>
-      <c r="N7" s="65"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="82"/>
+      <c r="M7" s="82"/>
+      <c r="N7" s="82"/>
       <c r="O7" s="14"/>
       <c r="P7" s="9"/>
     </row>
@@ -1790,15 +1605,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C8),ISBLANK(D8)),"Completar",IF(D8&gt;=C8,D8-C8,"Error")),"Error")</f>
         <v>1.9444444444444375E-2</v>
       </c>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="66"/>
-      <c r="N8" s="66"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="64"/>
+      <c r="N8" s="64"/>
       <c r="O8" s="15"/>
       <c r="P8" s="11"/>
     </row>
@@ -1822,26 +1637,26 @@
     </row>
     <row r="10" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="56"/>
-      <c r="M10" s="56"/>
-      <c r="N10" s="57"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="62"/>
+      <c r="L10" s="62"/>
+      <c r="M10" s="62"/>
+      <c r="N10" s="63"/>
       <c r="O10" s="13"/>
     </row>
     <row r="11" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="65" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="76" t="s">
@@ -1849,23 +1664,23 @@
       </c>
       <c r="D11" s="76"/>
       <c r="E11" s="77"/>
-      <c r="F11" s="61" t="s">
+      <c r="F11" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="62"/>
-      <c r="H11" s="63" t="s">
+      <c r="G11" s="79"/>
+      <c r="H11" s="75" t="s">
         <v>14</v>
       </c>
       <c r="I11" s="76"/>
       <c r="J11" s="77"/>
-      <c r="K11" s="61" t="s">
+      <c r="K11" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="L11" s="62"/>
-      <c r="M11" s="63" t="s">
+      <c r="L11" s="79"/>
+      <c r="M11" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="64" t="s">
+      <c r="N11" s="81" t="s">
         <v>2</v>
       </c>
       <c r="O11" s="14"/>
@@ -1873,7 +1688,7 @@
     </row>
     <row r="12" spans="1:16" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
-      <c r="B12" s="82"/>
+      <c r="B12" s="65"/>
       <c r="C12" s="76"/>
       <c r="D12" s="76"/>
       <c r="E12" s="77"/>
@@ -1898,8 +1713,8 @@
       <c r="L12" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="M12" s="63"/>
-      <c r="N12" s="64"/>
+      <c r="M12" s="75"/>
+      <c r="N12" s="81"/>
       <c r="O12" s="14"/>
       <c r="P12" s="9"/>
     </row>
@@ -1909,11 +1724,11 @@
         <f>ROW($B13)-12</f>
         <v>1</v>
       </c>
-      <c r="C13" s="67" t="s">
+      <c r="C13" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="67"/>
-      <c r="E13" s="68"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="70"/>
       <c r="F13" s="47">
         <v>40</v>
       </c>
@@ -1952,11 +1767,11 @@
         <f t="shared" ref="B14:B15" si="0">ROW($B14)-12</f>
         <v>2</v>
       </c>
-      <c r="C14" s="67" t="s">
+      <c r="C14" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="67"/>
-      <c r="E14" s="68"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="70"/>
       <c r="F14" s="47">
         <v>50</v>
       </c>
@@ -1995,11 +1810,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="67"/>
-      <c r="E15" s="68"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="70"/>
       <c r="F15" s="47">
         <v>200</v>
       </c>
@@ -2023,7 +1838,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="M15" s="53">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="N15" s="25">
         <f t="shared" ref="N15:N20" si="4">IFERROR(IF(OR(J15="Completar",ISBLANK(L15)),"Completar",J15+L15),"Error")</f>
@@ -2038,11 +1853,11 @@
         <f>ROW($B16)-12</f>
         <v>4</v>
       </c>
-      <c r="C16" s="67" t="s">
+      <c r="C16" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="67"/>
-      <c r="E16" s="68"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="70"/>
       <c r="F16" s="47">
         <v>20</v>
       </c>
@@ -2081,11 +1896,11 @@
         <f>ROW($B17)-12</f>
         <v>5</v>
       </c>
-      <c r="C17" s="67" t="s">
+      <c r="C17" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="67"/>
-      <c r="E17" s="68"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="70"/>
       <c r="F17" s="47">
         <v>20</v>
       </c>
@@ -2124,11 +1939,11 @@
         <f>ROW($B18)-12</f>
         <v>6</v>
       </c>
-      <c r="C18" s="67" t="s">
+      <c r="C18" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="67"/>
-      <c r="E18" s="68"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="70"/>
       <c r="F18" s="47">
         <v>20</v>
       </c>
@@ -2166,11 +1981,11 @@
         <f>ROW($B19)-12</f>
         <v>7</v>
       </c>
-      <c r="C19" s="67" t="s">
+      <c r="C19" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="67"/>
-      <c r="E19" s="68"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="70"/>
       <c r="F19" s="47">
         <v>100</v>
       </c>
@@ -2198,11 +2013,11 @@
         <f>ROW($B20)-12</f>
         <v>8</v>
       </c>
-      <c r="C20" s="67" t="s">
+      <c r="C20" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="67"/>
-      <c r="E20" s="68"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="70"/>
       <c r="F20" s="47">
         <v>30</v>
       </c>
@@ -2237,12 +2052,12 @@
     </row>
     <row r="21" spans="1:16" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15"/>
-      <c r="B21" s="69" t="s">
+      <c r="B21" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="70"/>
-      <c r="D21" s="70"/>
-      <c r="E21" s="71"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="85"/>
       <c r="F21" s="26">
         <f>SUM(F13:F20)</f>
         <v>480</v>
@@ -2267,7 +2082,7 @@
       </c>
       <c r="M21" s="32">
         <f>SUM(M13:M20)</f>
-        <v>469</v>
+        <v>484</v>
       </c>
       <c r="N21" s="33" t="str">
         <f>IF(OR(COUNTIF(N13:N20,"Error")&gt;0,COUNTIF(N13:N20,"Completar")&gt;0),"Error",SUM(N13:N20))</f>
@@ -2294,12 +2109,12 @@
       <c r="O22" s="16"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="55" t="s">
+      <c r="B23" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="57"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="63"/>
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
@@ -2373,33 +2188,33 @@
       <c r="N26" s="16"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="56"/>
-      <c r="G27" s="56"/>
-      <c r="H27" s="56"/>
-      <c r="I27" s="56"/>
-      <c r="J27" s="56"/>
-      <c r="K27" s="56"/>
-      <c r="L27" s="56"/>
-      <c r="M27" s="56"/>
-      <c r="N27" s="57"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="62"/>
+      <c r="F27" s="62"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="62"/>
+      <c r="J27" s="62"/>
+      <c r="K27" s="62"/>
+      <c r="L27" s="62"/>
+      <c r="M27" s="62"/>
+      <c r="N27" s="63"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="58" t="s">
+      <c r="B28" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="59"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="72">
+      <c r="C28" s="57"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="71">
         <f>M21</f>
-        <v>469</v>
-      </c>
-      <c r="F28" s="73"/>
+        <v>484</v>
+      </c>
+      <c r="F28" s="72"/>
       <c r="G28" s="34"/>
       <c r="H28" s="35"/>
       <c r="I28" s="35"/>
@@ -2410,16 +2225,16 @@
       <c r="N28" s="38"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="58" t="s">
+      <c r="B29" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="59"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="74" t="str">
+      <c r="C29" s="57"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="73" t="str">
         <f>IF(M21=0,0,IFERROR(M21/(N21*24),"Error"))</f>
         <v>Error</v>
       </c>
-      <c r="F29" s="75"/>
+      <c r="F29" s="74"/>
       <c r="G29" s="36"/>
       <c r="H29" s="37"/>
       <c r="I29" s="37"/>
@@ -2430,16 +2245,16 @@
       <c r="N29" s="39"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="58" t="s">
+      <c r="B30" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="C30" s="59"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="72">
+      <c r="C30" s="57"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="71">
         <f>IF(K21=0,0,IFERROR(ROUNDUP(K21/(M21/100),0),"Error"))</f>
         <v>2</v>
       </c>
-      <c r="F30" s="73"/>
+      <c r="F30" s="72"/>
       <c r="G30" s="36"/>
       <c r="H30" s="37"/>
       <c r="I30" s="37"/>
@@ -2450,16 +2265,16 @@
       <c r="N30" s="39"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="58" t="s">
+      <c r="B31" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="59"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="78">
+      <c r="C31" s="57"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="54">
         <f>IF(K21=0,0,IFERROR(K21/M21,"Error"))</f>
-        <v>1.7057569296375266E-2</v>
-      </c>
-      <c r="F31" s="79"/>
+        <v>1.6528925619834711E-2</v>
+      </c>
+      <c r="F31" s="55"/>
       <c r="G31" s="36"/>
       <c r="H31" s="37"/>
       <c r="I31" s="37"/>
@@ -2470,11 +2285,11 @@
       <c r="N31" s="39"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="58" t="s">
+      <c r="B32" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="59"/>
-      <c r="D32" s="60"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="58"/>
       <c r="E32" s="43">
         <f>E4</f>
         <v>2.083333333333337E-2</v>
@@ -2493,11 +2308,11 @@
       <c r="N32" s="39"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="58" t="s">
+      <c r="B33" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="59"/>
-      <c r="D33" s="60"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="58"/>
       <c r="E33" s="43">
         <f>E8</f>
         <v>1.9444444444444375E-2</v>
@@ -2517,11 +2332,11 @@
     </row>
     <row r="34" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16"/>
-      <c r="B34" s="58" t="s">
+      <c r="B34" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="59"/>
-      <c r="D34" s="60"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="58"/>
       <c r="E34" s="43">
         <f>E25</f>
         <v>2.083333333333337E-2</v>
@@ -2541,11 +2356,11 @@
       <c r="O34" s="16"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="58" t="s">
+      <c r="B35" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="59"/>
-      <c r="D35" s="60"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="58"/>
       <c r="E35" s="43">
         <f>L21</f>
         <v>3.3333333333333333E-2</v>
@@ -2564,11 +2379,11 @@
       <c r="N35" s="39"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="58" t="s">
+      <c r="B36" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="59"/>
-      <c r="D36" s="60"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="58"/>
       <c r="E36" s="43" t="str">
         <f>J21</f>
         <v>Error</v>
@@ -2587,16 +2402,16 @@
       <c r="N36" s="39"/>
     </row>
     <row r="37" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="83" t="s">
+      <c r="B37" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="84"/>
-      <c r="D37" s="85"/>
-      <c r="E37" s="80" t="str">
+      <c r="C37" s="67"/>
+      <c r="D37" s="68"/>
+      <c r="E37" s="59" t="str">
         <f>IF(COUNTIF(E32:E36,"Error")=0,SUM(E32:E36),"Error")</f>
         <v>Error</v>
       </c>
-      <c r="F37" s="81"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="40"/>
       <c r="H37" s="41"/>
       <c r="I37" s="41"/>
@@ -2624,6 +2439,31 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="41">
+    <mergeCell ref="C1:N1"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="F7:N7"/>
+    <mergeCell ref="F8:N8"/>
+    <mergeCell ref="B10:N10"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="F3:N3"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="C11:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="E37:F37"/>
@@ -2640,37 +2480,12 @@
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="C14:E14"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="C11:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="C1:N1"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="F7:N7"/>
-    <mergeCell ref="F8:N8"/>
-    <mergeCell ref="B10:N10"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="F3:N3"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="11" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
TP4 para entragar listo
</commit_message>
<xml_diff>
--- a/TP4/Documentacion/Planilla de Metricas.xlsx
+++ b/TP4/Documentacion/Planilla de Metricas.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmartin\Desktop\progra\pa-group\TP4\Documentacion\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Métricas" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>Preparación de la Prueba</t>
   </si>
@@ -115,25 +120,16 @@
     <t>Matriz Simetrica</t>
   </si>
   <si>
-    <t>Grafo</t>
-  </si>
-  <si>
-    <t>Matula</t>
-  </si>
-  <si>
-    <t>WelshPowell</t>
-  </si>
-  <si>
-    <t>Secuencial Aleatorio</t>
-  </si>
-  <si>
     <t>Generador</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
     <t>Nodo</t>
+  </si>
+  <si>
+    <t>GrafoNDNP</t>
+  </si>
+  <si>
+    <t>Probador</t>
   </si>
 </sst>
 </file>
@@ -192,7 +188,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,12 +209,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -610,7 +600,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -618,13 +608,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -633,16 +620,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -660,224 +647,221 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="6" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -931,7 +915,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-AR"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1007,7 +991,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Métricas!$B$32:$D$36</c:f>
+              <c:f>Métricas!$B$29:$D$33</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1030,7 +1014,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Métricas!$E$32:$E$36</c:f>
+              <c:f>Métricas!$E$29:$E$33</c:f>
               <c:numCache>
                 <c:formatCode>[h]:mm</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1041,13 +1025,13 @@
                   <c:v>1.9444444444444375E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.083333333333337E-2</c:v>
+                  <c:v>2.430555555555558E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.3333333333333333E-2</c:v>
+                  <c:v>5.0694444444444445E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.1145833333333332</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1103,13 +1087,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>9527</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1175,7 +1159,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1210,7 +1194,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1419,99 +1403,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C13:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.140625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="1.140625" style="15" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" style="1" customWidth="1"/>
     <col min="3" max="11" width="11.42578125" style="1" customWidth="1"/>
     <col min="12" max="12" width="13" style="1" customWidth="1"/>
     <col min="13" max="14" width="11.42578125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="1.140625" style="16" customWidth="1"/>
+    <col min="15" max="15" width="1.140625" style="15" customWidth="1"/>
     <col min="16" max="16384" width="11.42578125" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="23" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="23" t="s">
+    <row r="1" spans="1:16" s="21" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="61" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="13"/>
-    </row>
-    <row r="3" spans="1:16" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="21" t="s">
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="12"/>
+    </row>
+    <row r="3" spans="1:16" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="82"/>
-      <c r="N3" s="82"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="9"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="8"/>
     </row>
     <row r="4" spans="1:16" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
-      <c r="B4" s="45">
+      <c r="A4" s="14"/>
+      <c r="B4" s="43">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="C4" s="46">
+      <c r="C4" s="44">
         <v>0.79166666666666663</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="44">
         <v>0.8125</v>
       </c>
-      <c r="E4" s="33">
+      <c r="E4" s="31">
         <f>IFERROR(IF(OR(ISBLANK(C4),ISBLANK(D4)),"Completar",IF(D4&gt;=C4,D4-C4,"Error")),"Error")</f>
         <v>2.083333333333337E-2</v>
       </c>
@@ -1524,84 +1508,84 @@
       <c r="L4" s="64"/>
       <c r="M4" s="64"/>
       <c r="N4" s="64"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="11"/>
-    </row>
-    <row r="5" spans="1:16" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="7"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="10"/>
+    </row>
+    <row r="5" spans="1:16" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="6"/>
     </row>
     <row r="6" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="61" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="13"/>
-    </row>
-    <row r="7" spans="1:16" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="21" t="s">
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="12"/>
+    </row>
+    <row r="7" spans="1:16" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
-      <c r="L7" s="82"/>
-      <c r="M7" s="82"/>
-      <c r="N7" s="82"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="9"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="63"/>
+      <c r="N7" s="63"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="8"/>
     </row>
     <row r="8" spans="1:16" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="45">
+      <c r="A8" s="14"/>
+      <c r="B8" s="43">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="C8" s="46">
+      <c r="C8" s="44">
         <v>0.86458333333333337</v>
       </c>
-      <c r="D8" s="46">
+      <c r="D8" s="44">
         <v>0.88402777777777775</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="31">
         <f>IFERROR(IF(OR(ISBLANK(C8),ISBLANK(D8)),"Completar",IF(D8&gt;=C8,D8-C8,"Error")),"Error")</f>
         <v>1.9444444444444375E-2</v>
       </c>
@@ -1614,607 +1598,549 @@
       <c r="L8" s="64"/>
       <c r="M8" s="64"/>
       <c r="N8" s="64"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="11"/>
-    </row>
-    <row r="9" spans="1:16" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="7"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="10"/>
+    </row>
+    <row r="9" spans="1:16" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="6"/>
     </row>
     <row r="10" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="61" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
-      <c r="N10" s="63"/>
-      <c r="O10" s="13"/>
-    </row>
-    <row r="11" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="65" t="s">
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="55"/>
+      <c r="O10" s="12"/>
+    </row>
+    <row r="11" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="76" t="s">
+      <c r="C11" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="76"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="78" t="s">
+      <c r="D11" s="74"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="79"/>
-      <c r="H11" s="75" t="s">
+      <c r="G11" s="60"/>
+      <c r="H11" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="76"/>
-      <c r="J11" s="77"/>
-      <c r="K11" s="78" t="s">
+      <c r="I11" s="74"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="L11" s="79"/>
-      <c r="M11" s="75" t="s">
+      <c r="L11" s="60"/>
+      <c r="M11" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="81" t="s">
+      <c r="N11" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="O11" s="14"/>
-      <c r="P11" s="9"/>
-    </row>
-    <row r="12" spans="1:16" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="65"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="18" t="s">
+      <c r="O11" s="13"/>
+      <c r="P11" s="8"/>
+    </row>
+    <row r="12" spans="1:16" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="80"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="18" t="s">
+      <c r="K12" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="L12" s="19" t="s">
+      <c r="L12" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="M12" s="75"/>
-      <c r="N12" s="81"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="9"/>
+      <c r="M12" s="61"/>
+      <c r="N12" s="62"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="8"/>
     </row>
     <row r="13" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="24">
+      <c r="A13" s="14"/>
+      <c r="B13" s="22">
         <f>ROW($B13)-12</f>
         <v>1</v>
       </c>
-      <c r="C13" s="69" t="s">
+      <c r="C13" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="69"/>
-      <c r="E13" s="70"/>
-      <c r="F13" s="47">
+      <c r="D13" s="65"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="45">
         <v>40</v>
       </c>
-      <c r="G13" s="48">
+      <c r="G13" s="46">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="H13" s="49">
+      <c r="H13" s="47">
         <v>0.8125</v>
       </c>
-      <c r="I13" s="50">
+      <c r="I13" s="48">
         <v>0.82361111111111107</v>
       </c>
-      <c r="J13" s="20">
+      <c r="J13" s="18">
         <f>IFERROR(IF(OR(ISBLANK(H13),ISBLANK(I13)),"Completar",IF(I13&gt;=H13,I13-H13,"Error")),"Error")</f>
         <v>1.1111111111111072E-2</v>
       </c>
-      <c r="K13" s="51">
+      <c r="K13" s="49">
         <v>3</v>
       </c>
-      <c r="L13" s="52">
+      <c r="L13" s="50">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="M13" s="53">
+      <c r="M13" s="51">
         <v>37</v>
       </c>
-      <c r="N13" s="25">
+      <c r="N13" s="23">
         <f>IFERROR(IF(OR(J13="Completar",ISBLANK(L13)),"Completar",J13+L13),"Error")</f>
         <v>2.1527777777777736E-2</v>
       </c>
-      <c r="O13" s="15"/>
-      <c r="P13" s="11"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="10"/>
     </row>
     <row r="14" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="24">
+      <c r="A14" s="14"/>
+      <c r="B14" s="22">
         <f t="shared" ref="B14:B15" si="0">ROW($B14)-12</f>
         <v>2</v>
       </c>
-      <c r="C14" s="69" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="69"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="47">
+      <c r="C14" s="65" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="65"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="45">
         <v>50</v>
       </c>
-      <c r="G14" s="48">
+      <c r="G14" s="46">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="H14" s="49">
+      <c r="H14" s="47">
         <v>0.59027777777777779</v>
       </c>
-      <c r="I14" s="50">
+      <c r="I14" s="48">
         <v>0.59722222222222221</v>
       </c>
-      <c r="J14" s="20">
+      <c r="J14" s="18">
         <f t="shared" ref="J14" si="1">IFERROR(IF(OR(ISBLANK(H14),ISBLANK(I14)),"Completar",IF(I14&gt;=H14,I14-H14,"Error")),"Error")</f>
         <v>6.9444444444444198E-3</v>
       </c>
-      <c r="K14" s="51">
+      <c r="K14" s="49">
         <v>1</v>
       </c>
-      <c r="L14" s="52">
+      <c r="L14" s="50">
         <v>2.0833333333333333E-3</v>
       </c>
-      <c r="M14" s="53">
+      <c r="M14" s="51">
         <v>63</v>
       </c>
-      <c r="N14" s="25">
+      <c r="N14" s="23">
         <f t="shared" ref="N14" si="2">IFERROR(IF(OR(J14="Completar",ISBLANK(L14)),"Completar",J14+L14),"Error")</f>
         <v>9.0277777777777526E-3</v>
       </c>
-      <c r="O14" s="15"/>
-      <c r="P14" s="11"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="10"/>
     </row>
     <row r="15" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="24">
+      <c r="A15" s="14"/>
+      <c r="B15" s="22">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C15" s="69" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="69"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="47">
+      <c r="C15" s="65" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="65"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="45">
         <v>200</v>
       </c>
-      <c r="G15" s="48">
+      <c r="G15" s="46">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="H15" s="49">
+      <c r="H15" s="47">
         <v>0.60416666666666663</v>
       </c>
-      <c r="I15" s="50">
+      <c r="I15" s="48">
         <v>0.65277777777777779</v>
       </c>
-      <c r="J15" s="20">
-        <f t="shared" ref="J15:J20" si="3">IFERROR(IF(OR(ISBLANK(H15),ISBLANK(I15)),"Completar",IF(I15&gt;=H15,I15-H15,"Error")),"Error")</f>
+      <c r="J15" s="18">
+        <f t="shared" ref="J15:J17" si="3">IFERROR(IF(OR(ISBLANK(H15),ISBLANK(I15)),"Completar",IF(I15&gt;=H15,I15-H15,"Error")),"Error")</f>
         <v>4.861111111111116E-2</v>
       </c>
-      <c r="K15" s="51">
+      <c r="K15" s="49">
         <v>4</v>
       </c>
-      <c r="L15" s="52">
+      <c r="L15" s="50">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="M15" s="53">
-        <v>277</v>
-      </c>
-      <c r="N15" s="25">
-        <f t="shared" ref="N15:N20" si="4">IFERROR(IF(OR(J15="Completar",ISBLANK(L15)),"Completar",J15+L15),"Error")</f>
+      <c r="M15" s="51">
+        <v>264</v>
+      </c>
+      <c r="N15" s="23">
+        <f t="shared" ref="N15:N17" si="4">IFERROR(IF(OR(J15="Completar",ISBLANK(L15)),"Completar",J15+L15),"Error")</f>
         <v>6.9444444444444489E-2</v>
       </c>
-      <c r="O15" s="15"/>
-      <c r="P15" s="11"/>
-    </row>
-    <row r="16" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="24">
+      <c r="O15" s="14"/>
+      <c r="P15" s="10"/>
+    </row>
+    <row r="16" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="22">
         <f>ROW($B16)-12</f>
         <v>4</v>
       </c>
-      <c r="C16" s="69" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="69"/>
-      <c r="E16" s="70"/>
-      <c r="F16" s="47">
-        <v>20</v>
-      </c>
-      <c r="G16" s="48">
-        <v>3.472222222222222E-3</v>
-      </c>
-      <c r="H16" s="49">
-        <v>0.84375</v>
-      </c>
-      <c r="I16" s="50">
-        <v>0.84722222222222221</v>
-      </c>
-      <c r="J16" s="20">
-        <f t="shared" ref="J16:J17" si="5">IFERROR(IF(OR(ISBLANK(H16),ISBLANK(I16)),"Completar",IF(I16&gt;=H16,I16-H16,"Error")),"Error")</f>
-        <v>3.4722222222222099E-3</v>
-      </c>
-      <c r="K16" s="51">
-        <v>0</v>
-      </c>
-      <c r="L16" s="52">
-        <v>0</v>
-      </c>
-      <c r="M16" s="53">
-        <v>19</v>
-      </c>
-      <c r="N16" s="25">
-        <f t="shared" ref="N16:N17" si="6">IFERROR(IF(OR(J16="Completar",ISBLANK(L16)),"Completar",J16+L16),"Error")</f>
-        <v>3.4722222222222099E-3</v>
-      </c>
-      <c r="O16" s="15"/>
-      <c r="P16" s="11"/>
+      <c r="C16" s="65" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="65"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="45">
+        <v>150</v>
+      </c>
+      <c r="G16" s="46">
+        <v>3.125E-2</v>
+      </c>
+      <c r="H16" s="47">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="I16" s="48">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="J16" s="18">
+        <f t="shared" ref="J16" si="5">IFERROR(IF(OR(ISBLANK(H16),ISBLANK(I16)),"Completar",IF(I16&gt;=H16,I16-H16,"Error")),"Error")</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="K16" s="49">
+        <v>6</v>
+      </c>
+      <c r="L16" s="50">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="M16" s="51">
+        <v>221</v>
+      </c>
+      <c r="N16" s="23">
+        <f t="shared" ref="N16" si="6">IFERROR(IF(OR(J16="Completar",ISBLANK(L16)),"Completar",J16+L16),"Error")</f>
+        <v>5.9027777777777742E-2</v>
+      </c>
+      <c r="O16" s="12"/>
     </row>
     <row r="17" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="24">
+      <c r="A17" s="13"/>
+      <c r="B17" s="22">
         <f>ROW($B17)-12</f>
         <v>5</v>
       </c>
-      <c r="C17" s="69" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="69"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="47">
-        <v>20</v>
-      </c>
-      <c r="G17" s="48">
-        <v>3.472222222222222E-3</v>
-      </c>
-      <c r="H17" s="49">
-        <v>0.84791666666666676</v>
-      </c>
-      <c r="I17" s="50">
-        <v>0.84930555555555554</v>
-      </c>
-      <c r="J17" s="20">
-        <f t="shared" si="5"/>
-        <v>1.3888888888887729E-3</v>
-      </c>
-      <c r="K17" s="51">
-        <v>0</v>
-      </c>
-      <c r="L17" s="52">
-        <v>0</v>
-      </c>
-      <c r="M17" s="53">
-        <v>27</v>
-      </c>
-      <c r="N17" s="25">
-        <f t="shared" si="6"/>
-        <v>1.3888888888887729E-3</v>
-      </c>
-      <c r="O17" s="14"/>
-      <c r="P17" s="17"/>
-    </row>
-    <row r="18" spans="1:16" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="B18" s="24">
-        <f>ROW($B18)-12</f>
-        <v>6</v>
-      </c>
-      <c r="C18" s="69" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="69"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="47">
-        <v>20</v>
-      </c>
-      <c r="G18" s="48">
-        <v>3.472222222222222E-3</v>
-      </c>
-      <c r="H18" s="49">
-        <v>0.85</v>
-      </c>
-      <c r="I18" s="50">
-        <v>0.85138888888888886</v>
-      </c>
-      <c r="J18" s="20">
-        <f t="shared" si="3"/>
-        <v>1.388888888888884E-3</v>
-      </c>
-      <c r="K18" s="51">
-        <v>0</v>
-      </c>
-      <c r="L18" s="52">
-        <v>0</v>
-      </c>
-      <c r="M18" s="53">
-        <v>26</v>
-      </c>
-      <c r="N18" s="25">
-        <f t="shared" si="4"/>
-        <v>1.388888888888884E-3</v>
-      </c>
-      <c r="O18" s="16"/>
-    </row>
-    <row r="19" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="24">
-        <f>ROW($B19)-12</f>
-        <v>7</v>
-      </c>
-      <c r="C19" s="69" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="69"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="47">
+      <c r="C17" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="65"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="45">
         <v>100</v>
       </c>
-      <c r="G19" s="48">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="H19" s="49"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="20" t="str">
-        <f t="shared" ref="J19" si="7">IFERROR(IF(OR(ISBLANK(H19),ISBLANK(I19)),"Completar",IF(I19&gt;=H19,I19-H19,"Error")),"Error")</f>
-        <v>Completar</v>
-      </c>
-      <c r="K19" s="51"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="53"/>
-      <c r="N19" s="25" t="str">
-        <f t="shared" ref="N19" si="8">IFERROR(IF(OR(J19="Completar",ISBLANK(L19)),"Completar",J19+L19),"Error")</f>
-        <v>Completar</v>
-      </c>
-      <c r="O19" s="13"/>
-    </row>
-    <row r="20" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="24">
-        <f>ROW($B20)-12</f>
-        <v>8</v>
-      </c>
-      <c r="C20" s="69" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="69"/>
-      <c r="E20" s="70"/>
-      <c r="F20" s="47">
-        <v>30</v>
-      </c>
-      <c r="G20" s="48">
+      <c r="G17" s="46">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="H20" s="49">
+      <c r="H17" s="47">
         <v>0.49305555555555558</v>
       </c>
-      <c r="I20" s="50">
+      <c r="I17" s="48">
         <v>0.4993055555555555</v>
       </c>
-      <c r="J20" s="20">
+      <c r="J17" s="18">
         <f t="shared" si="3"/>
         <v>6.2499999999999223E-3</v>
       </c>
-      <c r="K20" s="51">
+      <c r="K17" s="49">
         <v>0</v>
       </c>
-      <c r="L20" s="52">
+      <c r="L17" s="50">
         <v>0</v>
       </c>
-      <c r="M20" s="53">
-        <v>35</v>
-      </c>
-      <c r="N20" s="25">
+      <c r="M17" s="51">
+        <v>157</v>
+      </c>
+      <c r="N17" s="23">
         <f t="shared" si="4"/>
         <v>6.2499999999999223E-3</v>
       </c>
-      <c r="O20" s="14"/>
-      <c r="P20" s="9"/>
-    </row>
-    <row r="21" spans="1:16" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="15"/>
-      <c r="B21" s="83" t="s">
+      <c r="O17" s="13"/>
+      <c r="P17" s="8"/>
+    </row>
+    <row r="18" spans="1:16" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="14"/>
+      <c r="B18" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="84"/>
-      <c r="D21" s="84"/>
-      <c r="E21" s="85"/>
-      <c r="F21" s="26">
-        <f>SUM(F13:F20)</f>
-        <v>480</v>
-      </c>
-      <c r="G21" s="27">
-        <f>SUM(G13:G20)</f>
+      <c r="C18" s="68"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="24">
+        <f>SUM(F13:F17)</f>
+        <v>540</v>
+      </c>
+      <c r="G18" s="25">
+        <f>SUM(G13:G17)</f>
         <v>0.10069444444444445</v>
       </c>
-      <c r="H21" s="28"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="30" t="str">
-        <f>IF(OR(COUNTIF(J13:J20,"Error")&gt;0,COUNTIF(J13:J20,"Completar")&gt;0),"Error",SUM(J13:J20))</f>
-        <v>Error</v>
-      </c>
-      <c r="K21" s="31">
-        <f>SUM(K13:K20)</f>
-        <v>8</v>
-      </c>
-      <c r="L21" s="27">
-        <f>SUM(L13:L20)</f>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="M21" s="32">
-        <f>SUM(M13:M20)</f>
-        <v>484</v>
-      </c>
-      <c r="N21" s="33" t="str">
-        <f>IF(OR(COUNTIF(N13:N20,"Error")&gt;0,COUNTIF(N13:N20,"Completar")&gt;0),"Error",SUM(N13:N20))</f>
-        <v>Error</v>
-      </c>
-      <c r="O21" s="15"/>
-      <c r="P21" s="11"/>
-    </row>
-    <row r="22" spans="1:16" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="16"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="16"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="16"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="61" t="s">
+      <c r="H18" s="26"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="28">
+        <f>IF(OR(COUNTIF(J13:J17,"Error")&gt;0,COUNTIF(J13:J17,"Completar")&gt;0),"Error",SUM(J13:J17))</f>
+        <v>0.1145833333333332</v>
+      </c>
+      <c r="K18" s="29">
+        <f>SUM(K13:K17)</f>
+        <v>14</v>
+      </c>
+      <c r="L18" s="25">
+        <f>SUM(L13:L17)</f>
+        <v>5.0694444444444445E-2</v>
+      </c>
+      <c r="M18" s="30">
+        <f>SUM(M13:M17)</f>
+        <v>742</v>
+      </c>
+      <c r="N18" s="31">
+        <f>IF(OR(COUNTIF(N13:N17,"Error")&gt;0,COUNTIF(N13:N17,"Completar")&gt;0),"Error",SUM(N13:N17))</f>
+        <v>0.16527777777777763</v>
+      </c>
+      <c r="O18" s="14"/>
+      <c r="P18" s="10"/>
+    </row>
+    <row r="19" spans="1:16" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="15"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B20" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-    </row>
-    <row r="24" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="21" t="s">
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+    </row>
+    <row r="21" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E24" s="22" t="s">
+      <c r="E21" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-    </row>
-    <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="45">
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+    </row>
+    <row r="22" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="43">
         <v>1.7361111111111112E-2</v>
       </c>
-      <c r="C25" s="46">
+      <c r="C22" s="44">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D25" s="46">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="E25" s="33">
-        <f>IFERROR(IF(OR(ISBLANK(C25),ISBLANK(D25)),"Completar",IF(D25&gt;=C25,D25-C25,"Error")),"Error")</f>
-        <v>2.083333333333337E-2</v>
-      </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-    </row>
-    <row r="26" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
-      <c r="N26" s="16"/>
+      <c r="D22" s="44">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="E22" s="31">
+        <f>IFERROR(IF(OR(ISBLANK(C22),ISBLANK(D22)),"Completar",IF(D22&gt;=C22,D22-C22,"Error")),"Error")</f>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B24" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="54"/>
+      <c r="L24" s="54"/>
+      <c r="M24" s="54"/>
+      <c r="N24" s="55"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B25" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="57"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="70">
+        <f>M18</f>
+        <v>742</v>
+      </c>
+      <c r="F25" s="71"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="36"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B26" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="57"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="72">
+        <f>IF(M18=0,0,IFERROR(M18/(N18*24),"Error"))</f>
+        <v>187.05882352941194</v>
+      </c>
+      <c r="F26" s="73"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="35"/>
+      <c r="N26" s="37"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="61" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="62"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="62"/>
-      <c r="I27" s="62"/>
-      <c r="J27" s="62"/>
-      <c r="K27" s="62"/>
-      <c r="L27" s="62"/>
-      <c r="M27" s="62"/>
-      <c r="N27" s="63"/>
+      <c r="B27" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="57"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="70">
+        <f>IF(K18=0,0,IFERROR(ROUNDUP(K18/(M18/100),0),"Error"))</f>
+        <v>2</v>
+      </c>
+      <c r="F27" s="71"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="35"/>
+      <c r="K27" s="35"/>
+      <c r="L27" s="35"/>
+      <c r="M27" s="35"/>
+      <c r="N27" s="37"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B28" s="56" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C28" s="57"/>
       <c r="D28" s="58"/>
-      <c r="E28" s="71">
-        <f>M21</f>
-        <v>484</v>
-      </c>
-      <c r="F28" s="72"/>
+      <c r="E28" s="76">
+        <f>IF(K18=0,0,IFERROR(K18/M18,"Error"))</f>
+        <v>1.8867924528301886E-2</v>
+      </c>
+      <c r="F28" s="77"/>
       <c r="G28" s="34"/>
       <c r="H28" s="35"/>
       <c r="I28" s="35"/>
@@ -2222,228 +2148,191 @@
       <c r="K28" s="35"/>
       <c r="L28" s="35"/>
       <c r="M28" s="35"/>
-      <c r="N28" s="38"/>
+      <c r="N28" s="37"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B29" s="56" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C29" s="57"/>
       <c r="D29" s="58"/>
-      <c r="E29" s="73" t="str">
-        <f>IF(M21=0,0,IFERROR(M21/(N21*24),"Error"))</f>
-        <v>Error</v>
-      </c>
-      <c r="F29" s="74"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
-      <c r="K29" s="37"/>
-      <c r="L29" s="37"/>
-      <c r="M29" s="37"/>
-      <c r="N29" s="39"/>
+      <c r="E29" s="41">
+        <f>E4</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F29" s="42">
+        <f t="shared" ref="F29:F33" si="7">IF(E29="Completar",E29,IFERROR(E29/$E$34,"Error"))</f>
+        <v>9.063444108761351E-2</v>
+      </c>
+      <c r="G29" s="34"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="35"/>
+      <c r="L29" s="35"/>
+      <c r="M29" s="35"/>
+      <c r="N29" s="37"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B30" s="56" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C30" s="57"/>
       <c r="D30" s="58"/>
-      <c r="E30" s="71">
-        <f>IF(K21=0,0,IFERROR(ROUNDUP(K21/(M21/100),0),"Error"))</f>
-        <v>2</v>
-      </c>
-      <c r="F30" s="72"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="37"/>
-      <c r="L30" s="37"/>
-      <c r="M30" s="37"/>
-      <c r="N30" s="39"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E30" s="41">
+        <f>E8</f>
+        <v>1.9444444444444375E-2</v>
+      </c>
+      <c r="F30" s="42">
+        <f t="shared" si="7"/>
+        <v>8.4592145015105494E-2</v>
+      </c>
+      <c r="G30" s="34"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="35"/>
+      <c r="K30" s="35"/>
+      <c r="L30" s="35"/>
+      <c r="M30" s="35"/>
+      <c r="N30" s="37"/>
+    </row>
+    <row r="31" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="15"/>
       <c r="B31" s="56" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C31" s="57"/>
       <c r="D31" s="58"/>
-      <c r="E31" s="54">
-        <f>IF(K21=0,0,IFERROR(K21/M21,"Error"))</f>
-        <v>1.6528925619834711E-2</v>
-      </c>
-      <c r="F31" s="55"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="37"/>
-      <c r="J31" s="37"/>
-      <c r="K31" s="37"/>
-      <c r="L31" s="37"/>
-      <c r="M31" s="37"/>
-      <c r="N31" s="39"/>
+      <c r="E31" s="41">
+        <f>E22</f>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="F31" s="42">
+        <f>IF(E31="Completar",E31,IFERROR(E31/$E$34,"Error"))</f>
+        <v>0.10574018126888235</v>
+      </c>
+      <c r="G31" s="34"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="35"/>
+      <c r="K31" s="35"/>
+      <c r="L31" s="35"/>
+      <c r="M31" s="35"/>
+      <c r="N31" s="37"/>
+      <c r="O31" s="15"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B32" s="56" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C32" s="57"/>
       <c r="D32" s="58"/>
-      <c r="E32" s="43">
-        <f>E4</f>
-        <v>2.083333333333337E-2</v>
-      </c>
-      <c r="F32" s="44" t="str">
-        <f t="shared" ref="F32:F36" si="9">IF(E32="Completar",E32,IFERROR(E32/$E$37,"Error"))</f>
-        <v>Error</v>
-      </c>
-      <c r="G32" s="36"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="37"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="37"/>
-      <c r="L32" s="37"/>
-      <c r="M32" s="37"/>
-      <c r="N32" s="39"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E32" s="41">
+        <f>L18</f>
+        <v>5.0694444444444445E-2</v>
+      </c>
+      <c r="F32" s="42">
+        <f t="shared" si="7"/>
+        <v>0.22054380664652581</v>
+      </c>
+      <c r="G32" s="34"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="35"/>
+      <c r="K32" s="35"/>
+      <c r="L32" s="35"/>
+      <c r="M32" s="35"/>
+      <c r="N32" s="37"/>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="56" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C33" s="57"/>
       <c r="D33" s="58"/>
-      <c r="E33" s="43">
-        <f>E8</f>
-        <v>1.9444444444444375E-2</v>
-      </c>
-      <c r="F33" s="44" t="str">
-        <f t="shared" si="9"/>
-        <v>Error</v>
-      </c>
-      <c r="G33" s="36"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="37"/>
-      <c r="L33" s="37"/>
-      <c r="M33" s="37"/>
-      <c r="N33" s="39"/>
-    </row>
-    <row r="34" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
-      <c r="B34" s="56" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="57"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="43">
-        <f>E25</f>
-        <v>2.083333333333337E-2</v>
-      </c>
-      <c r="F34" s="44" t="str">
-        <f>IF(E34="Completar",E34,IFERROR(E34/$E$37,"Error"))</f>
-        <v>Error</v>
-      </c>
-      <c r="G34" s="36"/>
-      <c r="H34" s="37"/>
-      <c r="I34" s="37"/>
-      <c r="J34" s="37"/>
-      <c r="K34" s="37"/>
-      <c r="L34" s="37"/>
-      <c r="M34" s="37"/>
-      <c r="N34" s="39"/>
-      <c r="O34" s="16"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="56" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="57"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="43">
-        <f>L21</f>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="F35" s="44" t="str">
-        <f t="shared" si="9"/>
-        <v>Error</v>
-      </c>
-      <c r="G35" s="36"/>
-      <c r="H35" s="37"/>
-      <c r="I35" s="37"/>
-      <c r="J35" s="37"/>
-      <c r="K35" s="37"/>
-      <c r="L35" s="37"/>
-      <c r="M35" s="37"/>
-      <c r="N35" s="39"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="C36" s="57"/>
-      <c r="D36" s="58"/>
-      <c r="E36" s="43" t="str">
-        <f>J21</f>
-        <v>Error</v>
-      </c>
-      <c r="F36" s="44" t="str">
-        <f t="shared" si="9"/>
-        <v>Error</v>
-      </c>
-      <c r="G36" s="36"/>
-      <c r="H36" s="37"/>
-      <c r="I36" s="37"/>
-      <c r="J36" s="37"/>
-      <c r="K36" s="37"/>
-      <c r="L36" s="37"/>
-      <c r="M36" s="37"/>
-      <c r="N36" s="39"/>
-    </row>
-    <row r="37" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="66" t="s">
+      <c r="E33" s="41">
+        <f>J18</f>
+        <v>0.1145833333333332</v>
+      </c>
+      <c r="F33" s="42">
+        <f t="shared" si="7"/>
+        <v>0.4984894259818729</v>
+      </c>
+      <c r="G33" s="34"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="37"/>
+    </row>
+    <row r="34" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="67"/>
-      <c r="D37" s="68"/>
-      <c r="E37" s="59" t="str">
-        <f>IF(COUNTIF(E32:E36,"Error")=0,SUM(E32:E36),"Error")</f>
-        <v>Error</v>
-      </c>
-      <c r="F37" s="60"/>
-      <c r="G37" s="40"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
-      <c r="J37" s="41"/>
-      <c r="K37" s="41"/>
-      <c r="L37" s="41"/>
-      <c r="M37" s="41"/>
-      <c r="N37" s="42"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="10"/>
-      <c r="M38" s="10"/>
-      <c r="N38" s="10"/>
+      <c r="C34" s="82"/>
+      <c r="D34" s="83"/>
+      <c r="E34" s="78">
+        <f>IF(COUNTIF(E29:E33,"Error")=0,SUM(E29:E33),"Error")</f>
+        <v>0.22986111111111096</v>
+      </c>
+      <c r="F34" s="79"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="39"/>
+      <c r="J34" s="39"/>
+      <c r="K34" s="39"/>
+      <c r="L34" s="39"/>
+      <c r="M34" s="39"/>
+      <c r="N34" s="40"/>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <mergeCells count="41">
+  <mergeCells count="38">
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="B24:N24"/>
+    <mergeCell ref="F4:N4"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="C11:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
     <mergeCell ref="C1:N1"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B25:D25"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="M11:M12"/>
     <mergeCell ref="N11:N12"/>
@@ -2451,35 +2340,9 @@
     <mergeCell ref="F8:N8"/>
     <mergeCell ref="B10:N10"/>
     <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="B18:E18"/>
     <mergeCell ref="F3:N3"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="C11:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="B27:N27"/>
-    <mergeCell ref="F4:N4"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C14:E14"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:XFD1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">

</xml_diff>